<commit_message>
completed communication tracker days gap
</commit_message>
<xml_diff>
--- a/public/Sample_Share_Certificate_Masters.xlsx
+++ b/public/Sample_Share_Certificate_Masters.xlsx
@@ -11,27 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>Instrument Type*</t>
-  </si>
-  <si>
-    <t>Endorsement</t>
-  </si>
-  <si>
-    <t>Endorsement Folio</t>
-  </si>
-  <si>
-    <t>Endorsement Date</t>
-  </si>
-  <si>
-    <t>Endorsement  Shareholder Name 1</t>
-  </si>
-  <si>
-    <t>Endorsement  Shareholder Name 2</t>
-  </si>
-  <si>
-    <t>Endorsement  Shareholder Name 3</t>
   </si>
   <si>
     <t>Company Master Id*</t>
@@ -1242,14 +1224,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="12.6719" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6719" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1259,114 +1241,42 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>